<commit_message>
Refactor Excel report generation in AllotedCountController; streamline data insertion, update cell references, and enhance template cleanup
</commit_message>
<xml_diff>
--- a/wwwroot/templates/actual_counts_template.xlsx
+++ b/wwwroot/templates/actual_counts_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rahul/projects/sewa/bhati-jatha-count-report/wwwroot/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52553111-D06B-AF4E-9B9D-6B1FFA9851E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FA938D-7FF5-5A45-9AE1-05CBFD41AA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8540" yWindow="500" windowWidth="29040" windowHeight="16000" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bhati-Sat" sheetId="18" r:id="rId1"/>
+    <sheet name="Bhati-Sewa-Count" sheetId="18" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -847,27 +847,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,95 +871,116 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,13 +1123,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1144,13 +1137,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1158,14 +1144,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1491,37 +1491,37 @@
     </row>
     <row r="2" spans="1:21" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="40" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="41"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="75"/>
     </row>
     <row r="3" spans="1:21" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="42" t="str">
+      <c r="B3" s="76" t="str">
         <f>_xlfn.CONCAT("DAY : ",TEXT(B2,"dddd"))</f>
         <v>DAY : Saturday</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="84"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="78"/>
       <c r="E3" s="13" t="s">
         <v>14</v>
       </c>
@@ -1564,11 +1564,11 @@
       <c r="R3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="44" t="s">
+      <c r="S3" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="45"/>
-      <c r="U3" s="46"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="81"/>
     </row>
     <row r="4" spans="1:21" s="6" customFormat="1" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1623,7 +1623,7 @@
       <c r="R4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="71" t="s">
+      <c r="S4" s="61" t="s">
         <v>6</v>
       </c>
       <c r="T4" s="20" t="s">
@@ -1637,8 +1637,8 @@
       <c r="A5" s="5"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="63"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="25"/>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -1650,12 +1650,12 @@
       <c r="N5" s="25"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="59">
+      <c r="Q5" s="45"/>
+      <c r="R5" s="50">
         <f>SUM(E5:Q5)</f>
         <v>0</v>
       </c>
-      <c r="S5" s="72">
+      <c r="S5" s="62">
         <f>SUM(E5:Q5)</f>
         <v>0</v>
       </c>
@@ -1663,7 +1663,7 @@
         <f>R5-S5</f>
         <v>0</v>
       </c>
-      <c r="U5" s="77" t="s">
+      <c r="U5" s="67" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1671,8 +1671,8 @@
       <c r="A6" s="5"/>
       <c r="B6" s="38"/>
       <c r="C6" s="29"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="64"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="55"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -1684,12 +1684,12 @@
       <c r="N6" s="28"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="53"/>
-      <c r="R6" s="60">
+      <c r="Q6" s="46"/>
+      <c r="R6" s="51">
         <f>SUM(E6:Q6)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="73">
+      <c r="S6" s="63">
         <f>SUM(E6:Q6)</f>
         <v>0</v>
       </c>
@@ -1697,14 +1697,14 @@
         <f>R6-S6</f>
         <v>0</v>
       </c>
-      <c r="U6" s="78"/>
+      <c r="U6" s="68"/>
     </row>
     <row r="7" spans="1:21" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="38"/>
       <c r="C7" s="29"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="64"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
@@ -1716,12 +1716,12 @@
       <c r="N7" s="28"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="60">
+      <c r="Q7" s="46"/>
+      <c r="R7" s="51">
         <f>SUM(E7:Q7)</f>
         <v>0</v>
       </c>
-      <c r="S7" s="73">
+      <c r="S7" s="63">
         <f>SUM(E7:Q7)</f>
         <v>0</v>
       </c>
@@ -1729,109 +1729,109 @@
         <f>R7-S7</f>
         <v>0</v>
       </c>
-      <c r="U7" s="78"/>
+      <c r="U7" s="68"/>
     </row>
     <row r="8" spans="1:21" s="6" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="61">
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="52">
         <f>SUM(E8:Q8)</f>
         <v>0</v>
       </c>
-      <c r="S8" s="74"/>
-      <c r="T8" s="51">
+      <c r="S8" s="64"/>
+      <c r="T8" s="44">
         <f>R8-S8</f>
         <v>0</v>
       </c>
-      <c r="U8" s="79"/>
+      <c r="U8" s="69"/>
     </row>
     <row r="9" spans="1:21" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="66">
+      <c r="C9" s="83"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="57">
         <f t="shared" ref="E9:T9" si="0">SUM(E5:E8)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="57">
+      <c r="I9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K9" s="57">
+      <c r="K9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L9" s="57">
+      <c r="L9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M9" s="57">
+      <c r="M9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N9" s="57">
+      <c r="N9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P9" s="57">
+      <c r="P9" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="58">
+      <c r="Q9" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R9" s="62">
+      <c r="R9" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S9" s="75">
+      <c r="S9" s="65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T9" s="76">
+      <c r="T9" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U9" s="80"/>
+      <c r="U9" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1872,33 +1872,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:R9">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="26" priority="2">
+      <formula>$E9&gt;#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="3">
+      <formula>$E9&lt;#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>$E9=#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="2">
-      <formula>$E9&gt;#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="3">
-      <formula>$E9&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G8">
-    <cfRule type="expression" dxfId="23" priority="48">
+    <cfRule type="expression" dxfId="23" priority="49">
+      <formula>$G5=#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="50">
+      <formula>$G5&gt;#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="48">
       <formula>$G5&lt;#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="49">
-      <formula>$G5=#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="50">
-      <formula>$G5&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H8">
-    <cfRule type="expression" dxfId="20" priority="51">
+    <cfRule type="expression" dxfId="20" priority="52">
+      <formula>$H5=#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="51">
       <formula>$H5&lt;#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="52">
-      <formula>$H5=#REF!</formula>
     </cfRule>
     <cfRule type="expression" dxfId="18" priority="53">
       <formula>$H5&gt;#REF!</formula>
@@ -1960,11 +1960,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:R8">
-    <cfRule type="expression" dxfId="2" priority="40">
+    <cfRule type="expression" dxfId="2" priority="41">
+      <formula>$R5&gt;#REF!</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="40">
       <formula>$R5=#REF!</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="41">
-      <formula>$R5&gt;#REF!</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="69">
       <formula>$R5&lt;#REF!</formula>

</xml_diff>